<commit_message>
Compatibility with standalone release.
</commit_message>
<xml_diff>
--- a/Data/RESULTS/ILI_GPKG_STATISTICS.xlsx
+++ b/Data/RESULTS/ILI_GPKG_STATISTICS.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,243 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Inhaber</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_km_durchgangsstrasse</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>kb_befreit</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodePers1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodePers2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodePers3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodePers4</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodePers5</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeOFG1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeOFG2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeOFG3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeOFG5</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeGW1</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeGW3</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeGW4</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeGW5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LU</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>365.898</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>346.457</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8.952</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7.513</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.971</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="I2" t="n">
+        <v>343.37</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8.132999999999999</v>
+      </c>
+      <c r="K2" t="n">
+        <v>14.39</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="M2" t="n">
+        <v>344.948</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4.605</v>
+      </c>
+      <c r="O2" t="n">
+        <v>16.34</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>344.233</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>333.885</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.685</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.463</v>
+      </c>
+      <c r="I3" t="n">
+        <v>335.28</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5.345</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2.145</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1.463</v>
+      </c>
+      <c r="M3" t="n">
+        <v>284.425</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.928</v>
+      </c>
+      <c r="O3" t="n">
+        <v>55.417</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.463</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BL</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>176.2151</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>162.7862</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.4289</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>131.8565</v>
+      </c>
+      <c r="J4" t="n">
+        <v>26.0675</v>
+      </c>
+      <c r="K4" t="n">
+        <v>18.2911</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>169.2787</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2.9284</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4.008</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code for granted .xlsx compatibility
</commit_message>
<xml_diff>
--- a/Data/RESULTS/ILI_GPKG_STATISTICS.xlsx
+++ b/Data/RESULTS/ILI_GPKG_STATISTICS.xlsx
@@ -461,52 +461,52 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>AmpelcodeOFG1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeOFG2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeOFG3</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeGW1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeGW3</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>AmpelcodeGW4</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>AmpelcodePers3</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>AmpelcodePers4</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>AmpelcodePers5</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>AmpelcodeOFG1</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>AmpelcodeOFG2</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>AmpelcodeOFG3</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>AmpelcodeOFG5</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>AmpelcodeGW1</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>AmpelcodeGW3</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>AmpelcodeGW4</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -518,148 +518,148 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LU</t>
+          <t>BL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>365.898</v>
+        <v>176.2151</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>346.457</v>
+        <v>162.7862</v>
       </c>
       <c r="E2" t="n">
-        <v>8.952</v>
+        <v>13.4289</v>
       </c>
       <c r="F2" t="n">
-        <v>7.513</v>
+        <v>131.8565</v>
       </c>
       <c r="G2" t="n">
-        <v>2.971</v>
+        <v>26.0675</v>
       </c>
       <c r="H2" t="n">
-        <v>0.005</v>
+        <v>18.2911</v>
       </c>
       <c r="I2" t="n">
-        <v>343.37</v>
+        <v>169.2787</v>
       </c>
       <c r="J2" t="n">
-        <v>8.132999999999999</v>
+        <v>2.9284</v>
       </c>
       <c r="K2" t="n">
-        <v>14.39</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="M2" t="n">
-        <v>344.948</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4.605</v>
-      </c>
-      <c r="O2" t="n">
-        <v>16.34</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.005</v>
-      </c>
+        <v>4.008</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>LU</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>344.233</v>
+        <v>365.898</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>333.885</v>
+        <v>346.457</v>
       </c>
       <c r="E3" t="n">
-        <v>6.685</v>
+        <v>8.952</v>
       </c>
       <c r="F3" t="n">
-        <v>1.66</v>
+        <v>343.37</v>
       </c>
       <c r="G3" t="n">
-        <v>0.54</v>
+        <v>8.132999999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>1.463</v>
+        <v>14.39</v>
       </c>
       <c r="I3" t="n">
-        <v>335.28</v>
+        <v>344.948</v>
       </c>
       <c r="J3" t="n">
-        <v>5.345</v>
+        <v>4.605</v>
       </c>
       <c r="K3" t="n">
-        <v>2.145</v>
+        <v>16.34</v>
       </c>
       <c r="L3" t="n">
-        <v>1.463</v>
+        <v>7.513</v>
       </c>
       <c r="M3" t="n">
-        <v>284.425</v>
+        <v>2.971</v>
       </c>
       <c r="N3" t="n">
-        <v>2.928</v>
+        <v>0.005</v>
       </c>
       <c r="O3" t="n">
-        <v>55.417</v>
+        <v>0.005</v>
       </c>
       <c r="P3" t="n">
-        <v>1.463</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BL</t>
+          <t>TG</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>176.2151</v>
+        <v>344.233</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>162.7862</v>
+        <v>333.885</v>
       </c>
       <c r="E4" t="n">
-        <v>13.4289</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+        <v>6.685</v>
+      </c>
+      <c r="F4" t="n">
+        <v>335.28</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5.345</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.145</v>
+      </c>
       <c r="I4" t="n">
-        <v>131.8565</v>
+        <v>284.425</v>
       </c>
       <c r="J4" t="n">
-        <v>26.0675</v>
+        <v>2.928</v>
       </c>
       <c r="K4" t="n">
-        <v>18.2911</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
+        <v>55.417</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1.66</v>
+      </c>
       <c r="M4" t="n">
-        <v>169.2787</v>
+        <v>0.54</v>
       </c>
       <c r="N4" t="n">
-        <v>2.9284</v>
+        <v>1.463</v>
       </c>
       <c r="O4" t="n">
-        <v>4.008</v>
-      </c>
-      <c r="P4" t="inlineStr"/>
+        <v>1.463</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.463</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>